<commit_message>
Update dashboard with new charts/data
</commit_message>
<xml_diff>
--- a/Summary of balances as at 25th Sep2025.xlsx
+++ b/Summary of balances as at 25th Sep2025.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\burie-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652B6D42-6B05-4D8B-9924-4DD180981623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD3F79C-0336-4464-A788-85281FF4D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="06.09.25" sheetId="2" r:id="rId1"/>
+    <sheet name="25-09-2025" sheetId="2" r:id="rId1"/>
     <sheet name="Overall Summary" sheetId="3" r:id="rId2"/>
     <sheet name="Monthly Deficits" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="77" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1528,7 +1528,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="2">
-        <v>16500</v>
+        <v>0</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="G16" s="65">
         <f t="shared" si="1"/>
-        <v>16500</v>
+        <v>0</v>
       </c>
       <c r="H16" s="61">
         <v>0</v>
@@ -1555,11 +1555,11 @@
       <c r="J16" s="6"/>
       <c r="K16" s="48">
         <f t="shared" si="0"/>
-        <v>16500</v>
+        <v>0</v>
       </c>
       <c r="L16" s="72">
         <f t="shared" si="2"/>
-        <v>16500</v>
+        <v>0</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="26"/>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19:N19" si="5">SUM(B3:B18)</f>
-        <v>223500</v>
+        <v>207000</v>
       </c>
       <c r="C19" s="46">
         <f t="shared" si="5"/>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="G19" s="30">
         <f t="shared" si="5"/>
-        <v>1106750</v>
+        <v>1090250</v>
       </c>
       <c r="H19" s="59">
         <f t="shared" si="5"/>
@@ -1699,11 +1699,11 @@
       </c>
       <c r="K19" s="49">
         <f t="shared" si="5"/>
-        <v>1121750</v>
+        <v>1105250</v>
       </c>
       <c r="L19" s="73">
         <f>SUM(L3:L18)</f>
-        <v>426750</v>
+        <v>410250</v>
       </c>
       <c r="M19" s="43">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
Updated Excel file with new sheet name
</commit_message>
<xml_diff>
--- a/Summary of balances as at 25th Sep2025.xlsx
+++ b/Summary of balances as at 25th Sep2025.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\burie-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD3F79C-0336-4464-A788-85281FF4D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0319827B-5AC4-485A-BDD2-F40D2F49349F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="25-09-2025" sheetId="2" r:id="rId1"/>
+    <sheet name="25.09.25" sheetId="2" r:id="rId1"/>
     <sheet name="Overall Summary" sheetId="3" r:id="rId2"/>
     <sheet name="Monthly Deficits" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -844,7 +844,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="77" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>